<commit_message>
Add the ability to import username and password for contacts.
</commit_message>
<xml_diff>
--- a/templates/Contacts.xlsx
+++ b/templates/Contacts.xlsx
@@ -33,8 +33,35 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>A list of valid email message categories, separated by comma. Valid categories are 2 for financial, 3 for general, 4 for services, 5 for outage notifications. </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If this is present, password must also be present. Minimum length is 5 character.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>If this is present, username must also be present. Minimum length is 8 characters.</t>
         </r>
       </text>
     </comment>
@@ -43,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Account ID</t>
   </si>
@@ -73,6 +100,12 @@
   </si>
   <si>
     <t>Email Message Categories</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -82,11 +115,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -113,12 +147,6 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -182,7 +210,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -192,10 +220,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -276,25 +300,25 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:colOff>27360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>753120</xdr:colOff>
+      <xdr:colOff>779760</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>143280</xdr:rowOff>
+      <xdr:rowOff>142920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="TextShape 1"/>
-        <xdr:cNvSpPr txBox="1"/>
+        <xdr:cNvPr id="0" name="CustomShape 1"/>
+        <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="360" y="0"/>
-          <a:ext cx="7255080" cy="5832720"/>
+          <a:off x="27360" y="0"/>
+          <a:ext cx="7153200" cy="5832360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -306,11 +330,22 @@
           <a:noFill/>
         </a:ln>
       </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0"/>
+        <a:fillRef idx="0"/>
+        <a:effectRef idx="0"/>
+        <a:fontRef idx="minor"/>
+      </xdr:style>
       <xdr:txBody>
         <a:bodyPr lIns="0" rIns="0" tIns="0" bIns="0"/>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>Importing contacts should be done using this sheet. The primary contact is imported using the 'Accounts' template, this is solely for secondary contacts.</a:t>
@@ -322,7 +357,29 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-US" sz="1200" spc="-1">
+            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Times New Roman"/>
+            </a:rPr>
+            <a:t>The username and password fields are for the customer portal. This requires Sonar version 0.6 or greater.</a:t>
+          </a:r>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:endParaRPr/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1200" spc="-1" strike="noStrike">
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
               <a:latin typeface="Times New Roman"/>
             </a:rPr>
             <a:t>All strings should be wrapped in double quotes (e.g. “Simon Westlake”)</a:t>
@@ -369,7 +426,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -388,25 +445,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="L1" activeCellId="0" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4285714285714"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9387755102041"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.4285714285714"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.8316326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6479591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5408163265306"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.2448979591837"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.9897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.7959183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.4948979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="16.0663265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="33.6122448979592"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="16.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -422,29 +480,35 @@
       <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>